<commit_message>
End of thursday, completed Patch (when successful) just deleting commented things
</commit_message>
<xml_diff>
--- a/Checklist_spreadsheet.xlsx
+++ b/Checklist_spreadsheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/isabelmaccabee/Documents/CODING/Northcoders/Back-End-02/BE2-NC-Knews/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A20BF19-6C5A-1C40-AA0E-F71ECD6134BC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDB93A52-2158-2A4D-B9FC-9EBA77FE9A3C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="460" windowWidth="27560" windowHeight="13960" xr2:uid="{C4E811DC-23B0-E24B-8C17-A553DFC04274}"/>
   </bookViews>
@@ -653,7 +653,7 @@
   <dimension ref="A2:K19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -908,8 +908,8 @@
       <c r="G10" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="H10" s="4" t="s">
-        <v>6</v>
+      <c r="H10" s="18" t="s">
+        <v>7</v>
       </c>
       <c r="I10" s="18" t="s">
         <v>7</v>

</xml_diff>

<commit_message>
Tests for defaula nd queries for getting comments bya article_id
</commit_message>
<xml_diff>
--- a/Checklist_spreadsheet.xlsx
+++ b/Checklist_spreadsheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/isabelmaccabee/Documents/CODING/Northcoders/Back-End-02/BE2-NC-Knews/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCA6F9B7-0A6B-5840-A783-3B4AC6B95210}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91E327DC-8D36-0144-AFAE-90F59E0A0138}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="460" windowWidth="27560" windowHeight="13960" xr2:uid="{C4E811DC-23B0-E24B-8C17-A553DFC04274}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="29">
   <si>
     <t>Successful</t>
   </si>
@@ -109,6 +109,9 @@
   </si>
   <si>
     <t>done (ish)</t>
+  </si>
+  <si>
+    <t>done (not defaults)</t>
   </si>
 </sst>
 </file>
@@ -653,7 +656,7 @@
   <dimension ref="A2:K19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -957,8 +960,12 @@
       <c r="B12" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="C12" s="18"/>
-      <c r="D12" s="12"/>
+      <c r="C12" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="D12" s="15" t="s">
+        <v>7</v>
+      </c>
       <c r="E12" s="12"/>
       <c r="F12" s="12"/>
       <c r="G12" s="12"/>
@@ -1021,8 +1028,8 @@
       <c r="B16" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="C16" s="15" t="s">
-        <v>7</v>
+      <c r="C16" s="33" t="s">
+        <v>28</v>
       </c>
       <c r="D16" s="26" t="s">
         <v>25</v>
@@ -1051,8 +1058,8 @@
       <c r="B17" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="C17" s="15" t="s">
-        <v>7</v>
+      <c r="C17" s="33" t="s">
+        <v>28</v>
       </c>
       <c r="D17" s="21" t="s">
         <v>8</v>

</xml_diff>

<commit_message>
Added post comment by article_id functionality
</commit_message>
<xml_diff>
--- a/Checklist_spreadsheet.xlsx
+++ b/Checklist_spreadsheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/isabelmaccabee/Documents/CODING/Northcoders/Back-End-02/BE2-NC-Knews/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91E327DC-8D36-0144-AFAE-90F59E0A0138}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6996DAD7-BEFD-6D41-8183-198E5E686714}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="460" windowWidth="27560" windowHeight="13960" xr2:uid="{C4E811DC-23B0-E24B-8C17-A553DFC04274}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="29">
   <si>
     <t>Successful</t>
   </si>
@@ -656,7 +656,7 @@
   <dimension ref="A2:K19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -970,7 +970,9 @@
       <c r="F12" s="12"/>
       <c r="G12" s="12"/>
       <c r="H12" s="12"/>
-      <c r="I12" s="12"/>
+      <c r="I12" s="17" t="s">
+        <v>7</v>
+      </c>
       <c r="J12" s="12"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
@@ -980,13 +982,19 @@
       <c r="B13" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="C13" s="19"/>
-      <c r="D13" s="16"/>
+      <c r="C13" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="D13" s="13" t="s">
+        <v>5</v>
+      </c>
       <c r="E13" s="16"/>
       <c r="F13" s="16"/>
       <c r="G13" s="16"/>
       <c r="H13" s="16"/>
-      <c r="I13" s="16"/>
+      <c r="I13" s="17" t="s">
+        <v>7</v>
+      </c>
       <c r="J13" s="16"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Added 404 test for comment_id patch
</commit_message>
<xml_diff>
--- a/Checklist_spreadsheet.xlsx
+++ b/Checklist_spreadsheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/isabelmaccabee/Documents/CODING/Northcoders/Back-End-02/BE2-NC-Knews/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6996DAD7-BEFD-6D41-8183-198E5E686714}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18D16B0B-CD45-5843-924D-CB75E94E270B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="460" windowWidth="27560" windowHeight="13960" xr2:uid="{C4E811DC-23B0-E24B-8C17-A553DFC04274}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="30">
   <si>
     <t>Successful</t>
   </si>
@@ -112,13 +112,16 @@
   </si>
   <si>
     <t>done (not defaults)</t>
+  </si>
+  <si>
+    <t>??</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -141,8 +144,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -171,6 +181,12 @@
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE2EFDA"/>
+        <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
   </fills>
@@ -300,9 +316,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -337,6 +350,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -656,7 +672,7 @@
   <dimension ref="A2:K19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -669,19 +685,19 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="C2" s="31" t="s">
+      <c r="C2" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="32"/>
-      <c r="E2" s="32"/>
-      <c r="F2" s="30" t="s">
+      <c r="D2" s="31"/>
+      <c r="E2" s="31"/>
+      <c r="F2" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="30"/>
-      <c r="H2" s="30"/>
-      <c r="I2" s="30"/>
-      <c r="J2" s="30"/>
-      <c r="K2" s="28"/>
+      <c r="G2" s="29"/>
+      <c r="H2" s="29"/>
+      <c r="I2" s="29"/>
+      <c r="J2" s="29"/>
+      <c r="K2" s="27"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B3" s="3"/>
@@ -709,7 +725,7 @@
       <c r="J3" s="9">
         <v>422</v>
       </c>
-      <c r="K3" s="27">
+      <c r="K3" s="26">
         <v>500</v>
       </c>
     </row>
@@ -723,7 +739,7 @@
       <c r="C4" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="26" t="s">
+      <c r="D4" s="25" t="s">
         <v>25</v>
       </c>
       <c r="E4" s="12"/>
@@ -753,7 +769,7 @@
       <c r="C5" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="26" t="s">
+      <c r="D5" s="25" t="s">
         <v>25</v>
       </c>
       <c r="E5" s="16"/>
@@ -774,7 +790,7 @@
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A6" s="24" t="s">
+      <c r="A6" s="23" t="s">
         <v>12</v>
       </c>
       <c r="B6" s="10" t="s">
@@ -786,11 +802,11 @@
       <c r="D6" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="E6" s="29"/>
+      <c r="E6" s="28"/>
       <c r="F6" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="G6" s="26" t="s">
+      <c r="G6" s="25" t="s">
         <v>25</v>
       </c>
       <c r="H6" s="13" t="s">
@@ -820,7 +836,7 @@
       <c r="F7" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="G7" s="26" t="s">
+      <c r="G7" s="25" t="s">
         <v>25</v>
       </c>
       <c r="H7" s="17" t="s">
@@ -829,15 +845,15 @@
       <c r="I7" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="J7" s="26" t="s">
+      <c r="J7" s="25" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A8" s="25" t="s">
+      <c r="A8" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="20" t="s">
+      <c r="B8" s="19" t="s">
         <v>18</v>
       </c>
       <c r="C8" s="15" t="s">
@@ -846,14 +862,14 @@
       <c r="D8" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="E8" s="21"/>
+      <c r="E8" s="20"/>
       <c r="F8" s="13" t="s">
         <v>5</v>
       </c>
       <c r="G8" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="H8" s="21" t="s">
+      <c r="H8" s="20" t="s">
         <v>8</v>
       </c>
       <c r="I8" s="17" t="s">
@@ -864,7 +880,7 @@
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A9" s="24" t="s">
+      <c r="A9" s="23" t="s">
         <v>12</v>
       </c>
       <c r="B9" s="10" t="s">
@@ -897,10 +913,10 @@
       <c r="A10" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="22" t="s">
+      <c r="B10" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="C10" s="33" t="s">
+      <c r="C10" s="32" t="s">
         <v>26</v>
       </c>
       <c r="D10" s="13" t="s">
@@ -954,7 +970,7 @@
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A12" s="24" t="s">
+      <c r="A12" s="23" t="s">
         <v>12</v>
       </c>
       <c r="B12" s="10" t="s">
@@ -967,13 +983,17 @@
         <v>7</v>
       </c>
       <c r="E12" s="12"/>
-      <c r="F12" s="12"/>
+      <c r="F12" s="13" t="s">
+        <v>5</v>
+      </c>
       <c r="G12" s="12"/>
       <c r="H12" s="12"/>
       <c r="I12" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="J12" s="12"/>
+      <c r="J12" s="34" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
@@ -995,23 +1015,35 @@
       <c r="I13" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="J13" s="16"/>
+      <c r="J13" s="16" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A14" s="24" t="s">
+      <c r="A14" s="23" t="s">
         <v>14</v>
       </c>
       <c r="B14" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="C14" s="18"/>
-      <c r="D14" s="12"/>
+      <c r="C14" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="D14" s="13" t="s">
+        <v>5</v>
+      </c>
       <c r="E14" s="12"/>
       <c r="F14" s="12"/>
       <c r="G14" s="12"/>
-      <c r="H14" s="12"/>
-      <c r="I14" s="12"/>
-      <c r="J14" s="12"/>
+      <c r="H14" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="I14" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="J14" s="25" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
@@ -1020,36 +1052,42 @@
       <c r="B15" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="C15" s="19"/>
+      <c r="C15" s="18"/>
       <c r="D15" s="16"/>
       <c r="E15" s="16"/>
-      <c r="F15" s="16"/>
+      <c r="F15" s="13" t="s">
+        <v>5</v>
+      </c>
       <c r="G15" s="16"/>
       <c r="H15" s="16"/>
-      <c r="I15" s="16"/>
-      <c r="J15" s="16"/>
+      <c r="I15" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="J15" s="25" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A16" s="25" t="s">
+      <c r="A16" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="B16" s="23" t="s">
+      <c r="B16" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="C16" s="33" t="s">
+      <c r="C16" s="32" t="s">
         <v>28</v>
       </c>
-      <c r="D16" s="26" t="s">
+      <c r="D16" s="25" t="s">
         <v>25</v>
       </c>
-      <c r="E16" s="21"/>
+      <c r="E16" s="20"/>
       <c r="F16" s="13" t="s">
         <v>5</v>
       </c>
       <c r="G16" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="H16" s="21" t="s">
+      <c r="H16" s="20" t="s">
         <v>8</v>
       </c>
       <c r="I16" s="15" t="s">
@@ -1060,19 +1098,19 @@
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A17" s="25" t="s">
+      <c r="A17" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="B17" s="23" t="s">
+      <c r="B17" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="C17" s="33" t="s">
+      <c r="C17" s="32" t="s">
         <v>28</v>
       </c>
-      <c r="D17" s="21" t="s">
+      <c r="D17" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="E17" s="21"/>
+      <c r="E17" s="20"/>
       <c r="F17" s="13" t="s">
         <v>5</v>
       </c>
@@ -1096,7 +1134,7 @@
       <c r="B18" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C18" s="34" t="s">
+      <c r="C18" s="33" t="s">
         <v>6</v>
       </c>
       <c r="D18" s="6" t="s">

</xml_diff>

<commit_message>
Completed DELETE success and 404 for delete
</commit_message>
<xml_diff>
--- a/Checklist_spreadsheet.xlsx
+++ b/Checklist_spreadsheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/isabelmaccabee/Documents/CODING/Northcoders/Back-End-02/BE2-NC-Knews/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18D16B0B-CD45-5843-924D-CB75E94E270B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5E5DF7F-DF9E-6A43-8453-10201A43934A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="460" windowWidth="27560" windowHeight="13960" xr2:uid="{C4E811DC-23B0-E24B-8C17-A553DFC04274}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="30">
   <si>
     <t>Successful</t>
   </si>
@@ -275,7 +275,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -314,9 +314,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
@@ -672,7 +669,7 @@
   <dimension ref="A2:K19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -685,19 +682,19 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="C2" s="30" t="s">
+      <c r="C2" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="31"/>
-      <c r="E2" s="31"/>
-      <c r="F2" s="29" t="s">
+      <c r="D2" s="30"/>
+      <c r="E2" s="30"/>
+      <c r="F2" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="29"/>
-      <c r="H2" s="29"/>
-      <c r="I2" s="29"/>
-      <c r="J2" s="29"/>
-      <c r="K2" s="27"/>
+      <c r="G2" s="28"/>
+      <c r="H2" s="28"/>
+      <c r="I2" s="28"/>
+      <c r="J2" s="28"/>
+      <c r="K2" s="26"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B3" s="3"/>
@@ -725,7 +722,7 @@
       <c r="J3" s="9">
         <v>422</v>
       </c>
-      <c r="K3" s="26">
+      <c r="K3" s="25">
         <v>500</v>
       </c>
     </row>
@@ -739,7 +736,7 @@
       <c r="C4" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="25" t="s">
+      <c r="D4" s="24" t="s">
         <v>25</v>
       </c>
       <c r="E4" s="12"/>
@@ -769,7 +766,7 @@
       <c r="C5" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="25" t="s">
+      <c r="D5" s="24" t="s">
         <v>25</v>
       </c>
       <c r="E5" s="16"/>
@@ -790,7 +787,7 @@
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A6" s="23" t="s">
+      <c r="A6" s="22" t="s">
         <v>12</v>
       </c>
       <c r="B6" s="10" t="s">
@@ -802,11 +799,11 @@
       <c r="D6" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="E6" s="28"/>
+      <c r="E6" s="27"/>
       <c r="F6" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="G6" s="25" t="s">
+      <c r="G6" s="24" t="s">
         <v>25</v>
       </c>
       <c r="H6" s="13" t="s">
@@ -836,7 +833,7 @@
       <c r="F7" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="G7" s="25" t="s">
+      <c r="G7" s="24" t="s">
         <v>25</v>
       </c>
       <c r="H7" s="17" t="s">
@@ -845,15 +842,15 @@
       <c r="I7" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="J7" s="25" t="s">
+      <c r="J7" s="24" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A8" s="24" t="s">
+      <c r="A8" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="19" t="s">
+      <c r="B8" s="18" t="s">
         <v>18</v>
       </c>
       <c r="C8" s="15" t="s">
@@ -862,14 +859,14 @@
       <c r="D8" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="E8" s="20"/>
+      <c r="E8" s="19"/>
       <c r="F8" s="13" t="s">
         <v>5</v>
       </c>
       <c r="G8" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="H8" s="20" t="s">
+      <c r="H8" s="19" t="s">
         <v>8</v>
       </c>
       <c r="I8" s="17" t="s">
@@ -880,7 +877,7 @@
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A9" s="23" t="s">
+      <c r="A9" s="22" t="s">
         <v>12</v>
       </c>
       <c r="B9" s="10" t="s">
@@ -913,10 +910,10 @@
       <c r="A10" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="21" t="s">
+      <c r="B10" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="C10" s="32" t="s">
+      <c r="C10" s="31" t="s">
         <v>26</v>
       </c>
       <c r="D10" s="13" t="s">
@@ -970,7 +967,7 @@
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A12" s="23" t="s">
+      <c r="A12" s="22" t="s">
         <v>12</v>
       </c>
       <c r="B12" s="10" t="s">
@@ -991,7 +988,7 @@
       <c r="I12" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="J12" s="34" t="s">
+      <c r="J12" s="33" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1020,7 +1017,7 @@
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A14" s="23" t="s">
+      <c r="A14" s="22" t="s">
         <v>14</v>
       </c>
       <c r="B14" s="10" t="s">
@@ -1041,7 +1038,7 @@
       <c r="I14" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="J14" s="25" t="s">
+      <c r="J14" s="24" t="s">
         <v>25</v>
       </c>
     </row>
@@ -1052,42 +1049,48 @@
       <c r="B15" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="C15" s="18"/>
-      <c r="D15" s="16"/>
+      <c r="C15" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="D15" s="13" t="s">
+        <v>5</v>
+      </c>
       <c r="E15" s="16"/>
       <c r="F15" s="13" t="s">
         <v>5</v>
       </c>
       <c r="G15" s="16"/>
-      <c r="H15" s="16"/>
+      <c r="H15" s="17" t="s">
+        <v>7</v>
+      </c>
       <c r="I15" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="J15" s="25" t="s">
+      <c r="J15" s="24" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A16" s="24" t="s">
+      <c r="A16" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="B16" s="22" t="s">
+      <c r="B16" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="C16" s="32" t="s">
+      <c r="C16" s="31" t="s">
         <v>28</v>
       </c>
-      <c r="D16" s="25" t="s">
+      <c r="D16" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="E16" s="20"/>
+      <c r="E16" s="19"/>
       <c r="F16" s="13" t="s">
         <v>5</v>
       </c>
       <c r="G16" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="H16" s="20" t="s">
+      <c r="H16" s="19" t="s">
         <v>8</v>
       </c>
       <c r="I16" s="15" t="s">
@@ -1098,19 +1101,19 @@
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A17" s="24" t="s">
+      <c r="A17" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="B17" s="22" t="s">
+      <c r="B17" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="C17" s="32" t="s">
+      <c r="C17" s="31" t="s">
         <v>28</v>
       </c>
-      <c r="D17" s="20" t="s">
+      <c r="D17" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="E17" s="20"/>
+      <c r="E17" s="19"/>
       <c r="F17" s="13" t="s">
         <v>5</v>
       </c>
@@ -1134,7 +1137,7 @@
       <c r="B18" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C18" s="33" t="s">
+      <c r="C18" s="32" t="s">
         <v>6</v>
       </c>
       <c r="D18" s="6" t="s">

</xml_diff>

<commit_message>
Prepping for heroku hosting
</commit_message>
<xml_diff>
--- a/Checklist_spreadsheet.xlsx
+++ b/Checklist_spreadsheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/isabelmaccabee/Documents/CODING/Northcoders/Back-End-02/BE2-NC-Knews/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5E5DF7F-DF9E-6A43-8453-10201A43934A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CC140E1-30BF-E543-A5A7-64E32D7EC250}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="460" windowWidth="27560" windowHeight="13960" xr2:uid="{C4E811DC-23B0-E24B-8C17-A553DFC04274}"/>
+    <workbookView xWindow="1680" yWindow="2640" windowWidth="27560" windowHeight="13960" xr2:uid="{C4E811DC-23B0-E24B-8C17-A553DFC04274}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="31">
   <si>
     <t>Successful</t>
   </si>
@@ -115,6 +115,9 @@
   </si>
   <si>
     <t>??</t>
+  </si>
+  <si>
+    <t>each should have diff body ones</t>
   </si>
 </sst>
 </file>
@@ -275,7 +278,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -350,6 +353,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -666,10 +672,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{366617DD-9EDD-2C40-B7E1-AF529E7D4B2E}">
-  <dimension ref="A2:K19"/>
+  <dimension ref="A2:K20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1030,8 +1036,12 @@
         <v>5</v>
       </c>
       <c r="E14" s="12"/>
-      <c r="F14" s="12"/>
-      <c r="G14" s="12"/>
+      <c r="F14" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="G14" s="17" t="s">
+        <v>7</v>
+      </c>
       <c r="H14" s="17" t="s">
         <v>7</v>
       </c>
@@ -1059,7 +1069,9 @@
       <c r="F15" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="G15" s="16"/>
+      <c r="G15" s="17" t="s">
+        <v>7</v>
+      </c>
       <c r="H15" s="17" t="s">
         <v>7</v>
       </c>
@@ -1164,6 +1176,11 @@
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C19" s="5"/>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="F20" s="34" t="s">
+        <v>30</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>